<commit_message>
modified controller and protocol
</commit_message>
<xml_diff>
--- a/Code/protocol.xlsx
+++ b/Code/protocol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
   <si>
     <t>功能描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -194,10 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>消音/报警</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,10 +229,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>火情报告</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Data2</t>
   </si>
   <si>
@@ -285,12 +277,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>动作类型
-BIT1=1：烟感
-BIT0=1：温感</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>全开=0，半开=1，全关=2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,14 +290,6 @@
   <si>
     <t>Data1
 编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注：
-ID_NUM=0xPQ
-P：层号
-Q：编号
-P=0：整楼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -338,11 +316,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>控制器与控制器传输
-CANID=控制器ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>控制器至探测器传输（8B，不足补0）
 CANID=探测器ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -350,6 +323,45 @@
   <si>
     <t>探测器至控制器传输（8B，不足补0）
 CANID=探测器ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制器与控制器传输
+CANID=目的控制器ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探测器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动作类型
+BIT1=1：烟感
+BIT0=1：温感</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属控制器ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总线广播ID=0xC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>令牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1B令牌号=探测器编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -434,7 +446,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -442,64 +454,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,641 +836,665 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23:N23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="9" style="2" customWidth="1"/>
+    <col min="2" max="13" width="9" style="2"/>
+    <col min="14" max="14" width="12.375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="I1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="A1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="I1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-    </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="4" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="I5" s="4" t="s">
+      <c r="G4" s="15"/>
+      <c r="I4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="4" t="s">
+      <c r="K4" s="15"/>
+      <c r="L4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="I6" s="2" t="s">
+      <c r="G5" s="17"/>
+      <c r="I5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="I7" s="2" t="s">
+      <c r="G6" s="17"/>
+      <c r="I6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" s="18" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5" t="s">
+      <c r="L7" s="16"/>
+      <c r="M7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="N7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
+      <c r="L8" s="16"/>
+      <c r="M8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5" t="s">
+      <c r="L9" s="16"/>
+      <c r="M9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="8"/>
-    </row>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13" t="s">
+    <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="I18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+    </row>
+    <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="I21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:17" ht="72.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="I22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="26" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="L26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="L30" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="I19" s="14" t="s">
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:15" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-    </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-    </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="I22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="I23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="L27" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="6" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="L31" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-    </row>
-    <row r="32" spans="1:15" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-    </row>
-    <row r="33" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C36" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C37" s="7"/>
-    </row>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="29">
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A18:G20"/>
+    <mergeCell ref="I18:O20"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="I1:O3"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="M21:N21"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="L27:O29"/>
-    <mergeCell ref="L31:O32"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A1:G3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="I1:O3"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="A27:I29"/>
-    <mergeCell ref="A19:G21"/>
-    <mergeCell ref="I19:O21"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>